<commit_message>
I repeat: COOKING. ELiminated a bunch of wasted tables
</commit_message>
<xml_diff>
--- a/demodata/awards.xlsx
+++ b/demodata/awards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\FF\TRUFFLE\TRUFFLEdashGIT\demodata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Library/CloudStorage/GoogleDrive-rmaxsmth@gmail.com/My Drive/FF/TRUFFLE/TRUFFLEdashGIT/demodata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EB039B-ED9D-4860-BA05-68E7EB8C85F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876EF3DA-0669-2344-8EA4-6A7DAC971CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="269">
   <si>
     <t>Season</t>
   </si>
@@ -1111,21 +1111,21 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J268" sqref="J268"/>
+      <selection pane="bottomLeft" activeCell="E274" sqref="E274"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="36.25" customWidth="1"/>
-    <col min="6" max="6" width="26.375" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" customWidth="1"/>
     <col min="7" max="9" width="10.5" customWidth="1"/>
-    <col min="10" max="10" width="21.125" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" customWidth="1"/>
     <col min="11" max="28" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>265</v>
       </c>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>4</v>
       </c>
@@ -2072,7 +2072,7 @@
       </c>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>4</v>
       </c>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>4</v>
       </c>
@@ -2126,7 +2126,7 @@
       </c>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>4</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>4</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>4</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>4</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>4</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>4</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>4</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>4</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>4</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>4</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>4</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>4</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>4</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>4</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>4</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>4</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>4</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>4</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>4</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>4</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>4</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>4</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>4</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>4</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>4</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>4</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>4</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>4</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>4</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>4</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>4</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>4</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>4</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>4</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>4</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>4</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>4</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>4</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>4</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>4</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>4</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>4</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>4</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>4</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>4</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>4</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>4</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>4</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>4</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>4</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>4</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>4</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>4</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>4</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>4</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>4</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>4</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>4</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>4</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>4</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>4</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>4</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>4</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>4</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>4</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>4</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>4</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>4</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>4</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>4</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>4</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>4</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>4</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>4</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>4</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>4</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>4</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>4</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>4</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>4</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>4</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>4</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>4</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>4</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>4</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>4</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>4</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>4</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>4</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>4</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>4</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>4</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>4</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>4</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>4</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>4</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>4</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>4</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>4</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>4</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>4</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>4</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>4</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>4</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>4</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>4</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>4</v>
       </c>
@@ -4810,7 +4810,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>4</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>4</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>4</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>4</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>4</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>4</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>4</v>
       </c>
@@ -4962,7 +4962,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="164" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>4</v>
       </c>
@@ -4983,7 +4983,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>4</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>4</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>4</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>4</v>
       </c>
@@ -5067,7 +5067,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>4</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>4</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>4</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>4</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>4</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>4</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>4</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>4</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>4</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>4</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>4</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>4</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>4</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>4</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>4</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>4</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>4</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>4</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>4</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>4</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>4</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>4</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>4</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>4</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>4</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>4</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>4</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>4</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>4</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>4</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>4</v>
       </c>
@@ -5773,7 +5773,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>4</v>
       </c>
@@ -5794,7 +5794,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="201" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>4</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="202" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>4</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="203" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>4</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="204" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>4</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="205" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>4</v>
       </c>
@@ -5904,7 +5904,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>4</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>4</v>
       </c>
@@ -5956,7 +5956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="208" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>4</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="209" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>4</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="210" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>4</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="211" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>4</v>
       </c>
@@ -6060,7 +6060,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="212" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>4</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="213" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>4</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>4</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="215" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>4</v>
       </c>
@@ -6164,7 +6164,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="216" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>4</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="217" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>4</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="218" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>4</v>
       </c>
@@ -6227,7 +6227,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="219" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>4</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="220" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>4</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="221" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>4</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="222" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>4</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="223" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>4</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="224" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>4</v>
       </c>
@@ -6353,7 +6353,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="225" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>4</v>
       </c>
@@ -6374,7 +6374,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="226" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>4</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>4</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>4</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>4</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>4</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>4</v>
       </c>
@@ -6500,7 +6500,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>4</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>4</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>4</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>4</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>4</v>
       </c>
@@ -6620,7 +6620,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>4</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>4</v>
       </c>
@@ -6672,7 +6672,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>4</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>4</v>
       </c>
@@ -6724,7 +6724,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>4</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>4</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>4</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>4</v>
       </c>
@@ -6828,7 +6828,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>4</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>4</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>4</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="248" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>4</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="249" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>4</v>
       </c>
@@ -6933,7 +6933,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="250" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>4</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="251" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
         <v>4</v>
       </c>
@@ -6975,7 +6975,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="252" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>4</v>
       </c>
@@ -6996,7 +6996,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="253" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>4</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="254" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>4</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="255" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>4</v>
       </c>
@@ -7059,7 +7059,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="256" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>4</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="257" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>4</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="258" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>4</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="259" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>4</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="260" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>4</v>
       </c>
@@ -7164,7 +7164,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="261" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>4</v>
       </c>
@@ -7185,7 +7185,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="262" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
         <v>4</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="263" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>266</v>
       </c>
@@ -7219,9 +7219,7 @@
       <c r="D263" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E263" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="E263" s="1"/>
       <c r="F263" s="1" t="s">
         <v>268</v>
       </c>
@@ -7232,7 +7230,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="264" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>266</v>
       </c>
@@ -7245,9 +7243,7 @@
       <c r="D264" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E264" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="E264" s="1"/>
       <c r="F264" s="1" t="s">
         <v>268</v>
       </c>
@@ -7258,7 +7254,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="265" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>266</v>
       </c>
@@ -7271,9 +7267,7 @@
       <c r="D265" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E265" s="6" t="s">
-        <v>258</v>
-      </c>
+      <c r="E265" s="6"/>
       <c r="F265" s="1" t="s">
         <v>268</v>
       </c>
@@ -7284,7 +7278,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="266" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>266</v>
       </c>
@@ -7297,9 +7291,7 @@
       <c r="D266" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E266" s="1" t="s">
-        <v>239</v>
-      </c>
+      <c r="E266" s="1"/>
       <c r="F266" s="1" t="s">
         <v>268</v>
       </c>
@@ -7310,7 +7302,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="267" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
         <v>266</v>
       </c>
@@ -7323,9 +7315,7 @@
       <c r="D267" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E267" s="1" t="s">
-        <v>259</v>
-      </c>
+      <c r="E267" s="1"/>
       <c r="F267" s="1" t="s">
         <v>268</v>
       </c>
@@ -7336,7 +7326,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="268" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>266</v>
       </c>
@@ -7349,9 +7339,7 @@
       <c r="D268" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E268" s="6" t="s">
-        <v>260</v>
-      </c>
+      <c r="E268" s="6"/>
       <c r="F268" s="1" t="s">
         <v>268</v>
       </c>
@@ -7362,7 +7350,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="269" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>266</v>
       </c>
@@ -7375,9 +7363,7 @@
       <c r="D269" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E269" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="E269" s="6"/>
       <c r="F269" s="1" t="s">
         <v>268</v>
       </c>
@@ -7388,7 +7374,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
         <v>266</v>
       </c>
@@ -7401,9 +7387,7 @@
       <c r="D270" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E270" s="6" t="s">
-        <v>262</v>
-      </c>
+      <c r="E270" s="6"/>
       <c r="F270" s="1" t="s">
         <v>268</v>
       </c>
@@ -7414,7 +7398,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="271" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
         <v>266</v>
       </c>
@@ -7427,9 +7411,7 @@
       <c r="D271" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E271" s="6" t="s">
-        <v>263</v>
-      </c>
+      <c r="E271" s="6"/>
       <c r="F271" s="1" t="s">
         <v>268</v>
       </c>
@@ -7440,7 +7422,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="272" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
         <v>266</v>
       </c>
@@ -7453,9 +7435,7 @@
       <c r="D272" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E272" s="6" t="s">
-        <v>264</v>
-      </c>
+      <c r="E272" s="6"/>
       <c r="F272" s="1" t="s">
         <v>268</v>
       </c>
@@ -7466,7 +7446,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="273" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
         <v>266</v>
       </c>
@@ -7479,9 +7459,7 @@
       <c r="D273" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E273" s="6" t="s">
-        <v>260</v>
-      </c>
+      <c r="E273" s="6"/>
       <c r="F273" s="1" t="s">
         <v>268</v>
       </c>
@@ -7492,7 +7470,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="274" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>266</v>
       </c>
@@ -7514,7 +7492,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="275" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
         <v>266</v>
       </c>
@@ -7536,7 +7514,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="276" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>266</v>
       </c>
@@ -7558,7 +7536,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="277" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
         <v>266</v>
       </c>
@@ -7580,7 +7558,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="278" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>266</v>
       </c>
@@ -7602,7 +7580,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
         <v>266</v>
       </c>
@@ -7624,7 +7602,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="280" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>266</v>
       </c>
@@ -7646,7 +7624,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="281" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
         <v>266</v>
       </c>
@@ -7668,7 +7646,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="282" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
         <v>266</v>
       </c>
@@ -7690,7 +7668,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="283" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
         <v>266</v>
       </c>
@@ -7712,7 +7690,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="284" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
         <v>266</v>
       </c>
@@ -7734,7 +7712,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="285" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
         <v>266</v>
       </c>
@@ -7756,7 +7734,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="286" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
         <v>266</v>
       </c>
@@ -7778,7 +7756,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="287" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
         <v>266</v>
       </c>
@@ -7800,7 +7778,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="288" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>266</v>
       </c>
@@ -7822,7 +7800,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="289" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
         <v>266</v>
       </c>
@@ -7844,7 +7822,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="290" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
         <v>266</v>
       </c>
@@ -7866,7 +7844,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="291" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="s">
         <v>266</v>
       </c>
@@ -7888,715 +7866,715 @@
         <v>268</v>
       </c>
     </row>
-    <row r="292" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>